<commit_message>
Initializes 20 random points to an Excel file Calculate the distance between two points.
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -556,7 +556,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>-4,-4</t>
         </is>
       </c>
       <c r="E2" s="3" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>1,8</t>
+          <t>9,0</t>
         </is>
       </c>
       <c r="E3" s="3" t="n">
@@ -608,7 +608,7 @@
       <c r="C4" s="3" t="n"/>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>-4,2</t>
+          <t>-10,-2</t>
         </is>
       </c>
       <c r="E4" s="3" t="n"/>
@@ -621,7 +621,7 @@
       <c r="C5" s="3" t="n"/>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>7,-1</t>
+          <t>-3,5</t>
         </is>
       </c>
       <c r="E5" s="3" t="n"/>
@@ -634,7 +634,7 @@
       <c r="C6" s="3" t="n"/>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>5,-8</t>
+          <t>-6,-8</t>
         </is>
       </c>
       <c r="E6" s="3" t="n"/>
@@ -647,7 +647,7 @@
       <c r="C7" s="3" t="n"/>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>-7,-2</t>
+          <t>3,-9</t>
         </is>
       </c>
       <c r="E7" s="3" t="n"/>
@@ -660,7 +660,7 @@
       <c r="C8" s="3" t="n"/>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>0,7</t>
+          <t>8,4</t>
         </is>
       </c>
       <c r="E8" s="3" t="n"/>
@@ -673,7 +673,7 @@
       <c r="C9" s="3" t="n"/>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>7,4</t>
+          <t>-8,2</t>
         </is>
       </c>
       <c r="E9" s="3" t="n"/>
@@ -686,7 +686,7 @@
       <c r="C10" s="3" t="n"/>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>-2,-3</t>
+          <t>2,8</t>
         </is>
       </c>
       <c r="E10" s="3" t="n"/>
@@ -699,7 +699,7 @@
       <c r="C11" s="3" t="n"/>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>-7,-1</t>
+          <t>-9,-1</t>
         </is>
       </c>
       <c r="E11" s="3" t="n"/>
@@ -712,7 +712,7 @@
       <c r="C12" s="3" t="n"/>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>-3,9</t>
+          <t>2,5</t>
         </is>
       </c>
       <c r="E12" s="3" t="n"/>
@@ -725,7 +725,7 @@
       <c r="C13" s="3" t="n"/>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>-5,1</t>
+          <t>-4,-1</t>
         </is>
       </c>
       <c r="E13" s="3" t="n"/>
@@ -738,7 +738,7 @@
       <c r="C14" s="3" t="n"/>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>6,2</t>
+          <t>-7,-9</t>
         </is>
       </c>
       <c r="E14" s="3" t="n"/>
@@ -751,7 +751,7 @@
       <c r="C15" s="3" t="n"/>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>6,1</t>
+          <t>9,-4</t>
         </is>
       </c>
       <c r="E15" s="3" t="n"/>
@@ -764,7 +764,7 @@
       <c r="C16" s="3" t="n"/>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>7,1</t>
         </is>
       </c>
       <c r="E16" s="3" t="n"/>
@@ -777,7 +777,7 @@
       <c r="C17" s="3" t="n"/>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>-3,-8</t>
+          <t>8,-6</t>
         </is>
       </c>
       <c r="E17" s="3" t="n"/>
@@ -790,7 +790,7 @@
       <c r="C18" s="3" t="n"/>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>5,0</t>
+          <t>-5,4</t>
         </is>
       </c>
       <c r="E18" s="3" t="n"/>
@@ -803,7 +803,7 @@
       <c r="C19" s="3" t="n"/>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>-9,-3</t>
+          <t>8,2</t>
         </is>
       </c>
       <c r="E19" s="3" t="n"/>
@@ -816,7 +816,7 @@
       <c r="C20" s="3" t="n"/>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>-4,3</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="E20" s="3" t="n"/>
@@ -829,7 +829,7 @@
       <c r="C21" s="3" t="n"/>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>-10,-7</t>
+          <t>-4,-6</t>
         </is>
       </c>
       <c r="E21" s="3" t="n"/>

</xml_diff>

<commit_message>
Adding comment and inserting children's data into a dictionary
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Child" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Accompanier" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Car" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="time_travel" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="School" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -19,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,6 +32,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FFA9B7C6"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="177"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -52,8 +61,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -67,10 +77,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
     <dxf>
       <alignment horizontal="left" vertical="bottom"/>
     </dxf>
@@ -98,8 +109,51 @@
     <dxf>
       <alignment horizontal="left" vertical="bottom"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -172,16 +226,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Child" displayName="Child" ref="A1:G21" headerRowCount="1" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Child" displayName="Child" ref="A1:G21" headerRowCount="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:G21"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" name="first_name" dataDxfId="5"/>
-    <tableColumn id="3" name="lest_name" dataDxfId="4"/>
-    <tableColumn id="4" name="address" dataDxfId="3"/>
-    <tableColumn id="5" name="contacts" dataDxfId="2"/>
-    <tableColumn id="6" name="id_school" dataDxfId="1"/>
-    <tableColumn id="7" name="special_needs" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="first_name" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="lest_name" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="address" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="contacts" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="id_school" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="special_needs" dataDxfId="7" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -205,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Car" displayName="Car" ref="A1:F2" headerRowCount="1" totalsRowShown="0">
-  <autoFilter ref="A1:F2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Car" displayName="Car" ref="A1:F4" headerRowCount="1" totalsRowShown="0">
+  <autoFilter ref="A1:F4"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="car_type"/>
@@ -214,6 +268,20 @@
     <tableColumn id="4" name="cost_per_minute"/>
     <tableColumn id="5" name="capacity"/>
     <tableColumn id="6" name="wheelchair"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="School" displayName="School" ref="A1:E2" headerRowCount="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E2"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" name="Addres" dataDxfId="2"/>
+    <tableColumn id="4" name="Contacts" dataDxfId="1"/>
+    <tableColumn id="5" name="Time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -488,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -556,14 +624,16 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>-4,-4</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>528401211</v>
+          <t>8,1</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
       </c>
       <c r="F2" s="3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
@@ -587,254 +657,616 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>9,0</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>542356958</v>
+          <t>-5,6</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
       </c>
       <c r="F3" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>302962915</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Asher </t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Castro</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>-8,4</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>308035542</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anastasia </t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Afanasenko</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>2,-10</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>311177802</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christina </t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Kipnis</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>8,7</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>305251175</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Or </t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Levi</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>-1,-2</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n"/>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" s="3" t="n"/>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>-10,-2</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="n"/>
-      <c r="F4" s="3" t="n"/>
-      <c r="G4" s="3" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>-3,5</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="n"/>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n"/>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>-6,-8</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="n"/>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>3,-9</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="n"/>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n"/>
+      <c r="A8" s="3" t="n">
+        <v>308051846</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eyal </t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Basis</t>
+        </is>
+      </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>8,4</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
+          <t>1,-8</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n"/>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="3" t="n"/>
+      <c r="A9" s="3" t="n">
+        <v>312049950</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Molham </t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Halaby</t>
+        </is>
+      </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>-8,2</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="n"/>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="n"/>
+          <t>-8,-2</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n"/>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="3" t="n"/>
+      <c r="A10" s="3" t="n">
+        <v>308073899</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anan </t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Mshelh</t>
+        </is>
+      </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>2,8</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="n"/>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
+          <t>-8,-3</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n"/>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="3" t="n"/>
+      <c r="A11" s="3" t="n">
+        <v>318869187</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soaad </t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Amer</t>
+        </is>
+      </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>-9,-1</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="n"/>
-      <c r="F11" s="3" t="n"/>
-      <c r="G11" s="3" t="n"/>
+          <t>-2,9</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="3" t="n"/>
+      <c r="A12" s="3" t="n">
+        <v>205898513</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Asaf </t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Ben Shabat</t>
+        </is>
+      </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>2,5</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="n"/>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="3" t="n"/>
+          <t>3,-8</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n"/>
-      <c r="B13" s="3" t="n"/>
-      <c r="C13" s="3" t="n"/>
+      <c r="A13" s="3" t="n">
+        <v>318428158</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tal </t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Vakrat</t>
+        </is>
+      </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>-4,-1</t>
-        </is>
-      </c>
-      <c r="E13" s="3" t="n"/>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
+          <t>-2,-9</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n"/>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" s="3" t="n"/>
+      <c r="A14" s="3" t="n">
+        <v>316028364</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sami </t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Odeh</t>
+        </is>
+      </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>-7,-9</t>
-        </is>
-      </c>
-      <c r="E14" s="3" t="n"/>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
+          <t>-10,7</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="n"/>
-      <c r="B15" s="3" t="n"/>
-      <c r="C15" s="3" t="n"/>
+      <c r="A15" s="3" t="n">
+        <v>318294931</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shalev </t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Kubi</t>
+        </is>
+      </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>9,-4</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="n"/>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
+          <t>-1,2</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="n"/>
-      <c r="B16" s="3" t="n"/>
-      <c r="C16" s="3" t="n"/>
+      <c r="A16" s="3" t="n">
+        <v>305487936</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Avihai </t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Uksusman</t>
+        </is>
+      </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>7,1</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="n"/>
-      <c r="F16" s="3" t="n"/>
-      <c r="G16" s="3" t="n"/>
+          <t>-1,-9</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n"/>
-      <c r="B17" s="3" t="n"/>
-      <c r="C17" s="3" t="n"/>
+      <c r="A17" s="3" t="n">
+        <v>313227928</v>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aviv </t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Leder</t>
+        </is>
+      </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>8,-6</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="n"/>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
+          <t>-9,9</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n"/>
-      <c r="B18" s="3" t="n"/>
-      <c r="C18" s="3" t="n"/>
+      <c r="A18" s="3" t="n">
+        <v>205807308</v>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sariel </t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Sofer</t>
+        </is>
+      </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>-5,4</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="n"/>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="n"/>
+          <t>6,4</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="n"/>
-      <c r="B19" s="3" t="n"/>
-      <c r="C19" s="3" t="n"/>
+      <c r="A19" s="3" t="n">
+        <v>315891549</v>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Raz </t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Peretz</t>
+        </is>
+      </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>8,2</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="n"/>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
+          <t>-10,-4</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n"/>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="3" t="n"/>
+      <c r="A20" s="3" t="n">
+        <v>315060103</v>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dan </t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Kirshenbaum</t>
+        </is>
+      </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>5,0</t>
-        </is>
-      </c>
-      <c r="E20" s="3" t="n"/>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
+          <t>-2,-3</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="n"/>
-      <c r="B21" s="3" t="n"/>
-      <c r="C21" s="3" t="n"/>
+      <c r="A21" s="3" t="n">
+        <v>313925141</v>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Elad  </t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Leibovich</t>
+        </is>
+      </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>-4,-6</t>
-        </is>
-      </c>
-      <c r="E21" s="3" t="n"/>
-      <c r="F21" s="3" t="n"/>
-      <c r="G21" s="3" t="n"/>
+          <t>-8,-9</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n"/>
@@ -966,10 +1398,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1020,24 +1452,69 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>minibus</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>25</v>
       </c>
       <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
         <v>7</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>123</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>minibus</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>124</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>minibus</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1050,10 +1527,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A1" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1061,28 +1538,84 @@
     <col width="6.77734375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.109375" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="10" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>a_to_b</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>b_to_school</t>
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Addres</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B2" t="n">
-        <v>17</v>
+      <c r="A2" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Ironiah</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0,0</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change to openpyxl and creating school obj
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Child" sheetId="1" state="visible" r:id="rId1"/>
@@ -579,7 +579,7 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -647,7 +647,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>-8,2</t>
+          <t>9,-2</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>2,7</t>
+          <t>2,-1</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>-9,-3</t>
+          <t>-7,-3</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>-1,-1</t>
+          <t>8,6</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>-4,4</t>
+          <t>2,0</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>-3,-4</t>
+          <t>-3,5</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>1,7</t>
+          <t>2,-1</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>-9,0</t>
+          <t>8,3</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>-6,-2</t>
+          <t>-5,-10</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>-5,2</t>
+          <t>-9,-6</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
@@ -977,7 +977,7 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>-7,7</t>
+          <t>7,6</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>9,0</t>
+          <t>8,0</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>6,-1</t>
+          <t>3,5</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>-10,-2</t>
+          <t>5,-7</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>-9,-4</t>
+          <t>-4,9</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>-6,8</t>
+          <t>-7,-6</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>-7,6</t>
+          <t>0,-9</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>-3,-10</t>
+          <t>-3,-8</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>8,-2</t>
+          <t>-3,2</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>-2,-9</t>
+          <t>1,-2</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
@@ -1574,8 +1574,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
add func to div dictionary
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -647,7 +647,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>9,0</t>
+          <t>-10,8</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>6,5</t>
+          <t>-6,1</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>0,-5</t>
+          <t>-1,8</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>-9,5</t>
+          <t>-1,0</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>-8,-8</t>
+          <t>-6,-3</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>-6,-2</t>
+          <t>0,-1</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>4,-10</t>
+          <t>6,-9</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>-3,-9</t>
+          <t>5,-4</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>3,-1</t>
+          <t>5,1</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>5,3</t>
+          <t>-10,6</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
@@ -977,7 +977,7 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>-8,8</t>
+          <t>6,4</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>9,-7</t>
+          <t>4,1</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>4,-1</t>
+          <t>2,1</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>-5,2</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>-4,4</t>
+          <t>-2,-5</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>0,5</t>
+          <t>-9,-1</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>7,0</t>
+          <t>-8,2</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>1,-10</t>
+          <t>-4,7</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>-1,-1</t>
+          <t>1,-6</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>-4,6</t>
+          <t>8,0</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">

</xml_diff>

<commit_message>
fix bugs in "print_to_excel" and "calculate_time_cost_per_group"
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -647,7 +647,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>-2,7</t>
+          <t>-3,2</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>5,-1</t>
+          <t>-2,1</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>-6,-2</t>
+          <t>-10,-9</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>-5,-5</t>
+          <t>-3,0</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>5,2</t>
+          <t>-4,-1</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>-5,5</t>
+          <t>-10,1</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>-1,8</t>
+          <t>-1,7</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>-5,4</t>
+          <t>2,4</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>-8,2</t>
+          <t>-6,-9</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>-9,3</t>
+          <t>-4,-3</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
@@ -977,7 +977,7 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>-9,4</t>
+          <t>-7,1</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>-1,9</t>
+          <t>-7,-5</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>-3,0</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>0,-9</t>
+          <t>-3,7</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>-7,9</t>
+          <t>-5,-1</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>2,9</t>
+          <t>-8,-1</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>4,-3</t>
+          <t>-1,-8</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>1,5</t>
+          <t>7,8</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>9,-7</t>
+          <t>-3,-6</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>-8,-8</t>
+          <t>-8,8</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">

</xml_diff>